<commit_message>
rewrote sizing to class
</commit_message>
<xml_diff>
--- a/aircraft_inputs.xlsx
+++ b/aircraft_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiesh\TUDelft\MSc FP\Knowledge Based Engineering\KBE_transport_AC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C91DD9-F3D3-4DF9-977C-BBF1A83AF82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163855F3-2D39-4F6C-9222-71D403BB4140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>num_crates</t>
   </si>
@@ -75,9 +75,6 @@
     <t>AoA</t>
   </si>
   <si>
-    <t>mach</t>
-  </si>
-  <si>
     <t>Nz</t>
   </si>
   <si>
@@ -138,10 +135,19 @@
     <t>Input the required angle of attack in cruise conditions, in degrees</t>
   </si>
   <si>
-    <t>Input the Mach number at cruise conditions</t>
-  </si>
-  <si>
     <t>Input the ultimate load factor</t>
+  </si>
+  <si>
+    <t>Nt</t>
+  </si>
+  <si>
+    <t>Number of fuel tanks</t>
+  </si>
+  <si>
+    <t>eff_p</t>
+  </si>
+  <si>
+    <t>Propulsive efficiency</t>
   </si>
 </sst>
 </file>
@@ -476,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,10 +496,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -504,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -515,7 +521,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -526,7 +532,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -537,7 +543,7 @@
         <v>4000000</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -548,7 +554,7 @@
         <v>1093</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -559,7 +565,7 @@
         <v>975</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -570,7 +576,7 @@
         <v>8535</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -581,7 +587,7 @@
         <v>150</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -592,7 +598,7 @@
         <v>10.1</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -603,7 +609,7 @@
         <v>64318</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -614,7 +620,7 @@
         <v>64412</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -625,7 +631,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -636,7 +642,7 @@
         <v>0.4</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -644,10 +650,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
         <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -655,10 +661,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -669,7 +675,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -677,21 +683,32 @@
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>0.49</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commenting and extension of output file
</commit_message>
<xml_diff>
--- a/aircraft_inputs.xlsx
+++ b/aircraft_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiesh\TUDelft\MSc FP\Knowledge Based Engineering\KBE_transport_AC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163855F3-2D39-4F6C-9222-71D403BB4140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7F15BD-5778-4608-BB2D-564032C195B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>num_crates</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Propulsive efficiency</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>6000</t>
   </si>
 </sst>
 </file>
@@ -485,7 +491,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,8 +578,8 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
-        <v>8535</v>
+      <c r="B8" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -671,8 +677,8 @@
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3">
-        <v>2</v>
+      <c r="B17" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="C17" t="s">
         <v>35</v>

</xml_diff>